<commit_message>
Remove the score sort feature.
</commit_message>
<xml_diff>
--- a/sample/sorted.xlsx
+++ b/sample/sorted.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,8 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>M109
-6/16/22</t>
+          <t>Milestone/Release Due Date</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -517,37 +516,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2022-06-13</t>
+          <t>2022-06-14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sharry Xu</t>
+          <t>Mark Sun</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Develop Jira tool</t>
+          <t>[QA][Go-Live] Refund ATM Fees over 25% of credit limit in first year</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://jira.com/browse/proj-001</t>
+          <t>https://pd.nextestate.com/browse/GBOS-62337</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>M109</t>
+          <t>M111</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -557,7 +556,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -572,7 +571,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -582,117 +581,1681 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>2022-05-25</t>
+          <t>2022-06-23</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>2022-05-20</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Tyler Penn</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[Web] [GO2bank] [ODP 2.0] Go-Live (Desktop browser)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-37261</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2022-05-20</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tyler Penn</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[Web] [GO2bank] [ODP 2.0] Go-Live (Mobile browser)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-37262</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2022-05-20</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Tyler Penn</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[iOS/Android][GO2bank] [ODP 2.0] Go-Live</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BMAPP-21834</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2022-05-20</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tyler Penn</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[Automate] GO2bank ODP Fee Reversal</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GBOS-61531</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2022-06-02</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Tyler Penn</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ODP 2.0 : [TRIGGER FOR NTKey105] Tier Reinstated</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GBOS-62115</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2022-06-07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Smitha Jonnala</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[WMMC] OAuth redirect is not working as expected</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GB-80048</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2022-06-22</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Tyler Penn</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[Gateway] [GO2bank] [app upgrade] Set app force upgrade</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-38827</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2022-06-15</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Mark Sun</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[SCC] Block non-SSN DDA applying for an SCC</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GBOS-62345</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2022-05-23</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Megan Ackling</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[QA Testing]ATM and AFT Limit Decrease for Regular Season - CoID 164</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GBOS-62061</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2022-06-14</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Sarath Krishnan</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>[GFT]Update the Utility Core API to get Bin info to add Program code</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GBOS-62197</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2022-05-20</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Megan Ackling</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Walgreens and CVS FeeSplit Setup for eCash Setup - GBOS</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/FEAS-24667</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2022-06-06</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Sarath Krishnan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>[GFT][MCsend]Create Adjusmentypes for Partner A2A and P2P</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GBOS-61750</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>2022-06-13</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Andy Wu</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Review the design</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://jira.com/browse/proj-002</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>M109</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Critical</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>Critical</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>2022-05-25</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Rita Webb</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>[COFO]  Research Extensibility of Current Mobile 2FA Service</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>[GBOS-61873] [COFO][SPIKE] Research Extensibility of Current Mobile 2FA Service - GDCJira (nextestate.com)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2022-06-08</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Smitha Jonnala</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>BUX-37721: [Web] - [Server] [Go2bank and Chirp] Transactions API is not returning masked external account values for SCC transactions</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-37721</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2022-06-08</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Smitha Jonnala</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>BMAPP-21860: [Server] [Go2bank and Chirp] Transactions API is not returning masked external account values for SCC transactions</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BMAPP-21860</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2022-06-16</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Mark Sun</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>[QA ONLY] SCC declines can re-apply after 30 days</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BMAPP-22159</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2022-06-16</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Mark Sun</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>[QA only] SCC declines can re-apply after 30 days</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-38697</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2022-06-16</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Dennis Wiles</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>[GO2bank][Web] Add Domains to CSP Whitelisting</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-38699</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
         <is>
           <t>False</t>
         </is>

</xml_diff>

<commit_message>
Fix some bugs about the story class.
</commit_message>
<xml_diff>
--- a/sample/sorted.xlsx
+++ b/sample/sorted.xlsx
@@ -614,22 +614,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Tony Wei</t>
+          <t>John Rease</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sign Off</t>
+          <t>Testing</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://jira.com/browse/proj-005</t>
+          <t>https://jira.com/browse/proj-003</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>M110</t>
+          <t>M109</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -639,17 +639,17 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>High</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>High</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -798,22 +798,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>John Rease</t>
+          <t>Tony Wei</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Testing</t>
+          <t>Sign Off</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://jira.com/browse/proj-003</t>
+          <t>https://jira.com/browse/proj-005</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>M109</t>
+          <t>M110</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -823,17 +823,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>High</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">

</xml_diff>

<commit_message>
Re-implement the sort algorithm
</commit_message>
<xml_diff>
--- a/sample/sorted.xlsx
+++ b/sample/sorted.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,8 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>M109
-6/16/22</t>
+          <t>Milestone/Release Due Date</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -517,37 +516,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2022-06-13</t>
+          <t>2022-06-14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sharry Xu</t>
+          <t>Mark Sun</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Develop Jira tool</t>
+          <t>[QA][Go-Live] Refund ATM Fees over 25% of credit limit in first year</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://jira.com/browse/proj-001</t>
+          <t>https://pd.nextestate.com/browse/GBOS-62337</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>M109</t>
+          <t>M111</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -557,7 +556,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -572,7 +571,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -582,54 +581,54 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>2022-05-25</t>
+          <t>2022-06-23</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2022-06-13</t>
+          <t>2022-05-20</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>John Rease</t>
+          <t>Tyler Penn</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Testing</t>
+          <t>[Automate] GO2bank ODP Fee Reversal</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://jira.com/browse/proj-003</t>
+          <t>https://pd.nextestate.com/browse/GBOS-61531</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>M109</t>
+          <t>M111</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -644,12 +643,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -664,7 +663,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -674,17 +673,17 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>2022-05-25</t>
+          <t>2022-06-23</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -701,47 +700,47 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2022-06-13</t>
+          <t>2022-06-15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Andy Wu</t>
+          <t>Mark Sun</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Review the design</t>
+          <t>[SCC] Block non-SSN DDA applying for an SCC</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://jira.com/browse/proj-002</t>
+          <t>https://pd.nextestate.com/browse/GBOS-62345</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>M109</t>
+          <t>M111</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -756,27 +755,27 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>High</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>2022-05-25</t>
+          <t>2022-06-23</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -793,82 +792,82 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2022-06-13</t>
+          <t>2022-06-22</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tony Wei</t>
+          <t>Tyler Penn</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sign Off</t>
+          <t>[Gateway] [GO2bank] [app upgrade] Set app force upgrade</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://jira.com/browse/proj-005</t>
+          <t>https://pd.nextestate.com/browse/BUX-38827</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>M110</t>
+          <t>M111</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
           <t>True</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Critical</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>2022-05-25</t>
+          <t>2022-06-23</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -885,90 +884,1378 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>2022-05-20</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tyler Penn</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[Web] [GO2bank] [ODP 2.0] Go-Live (Desktop browser)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-37261</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2022-05-20</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Tyler Penn</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>[Web] [GO2bank] [ODP 2.0] Go-Live (Mobile browser)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-37262</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2022-05-20</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Tyler Penn</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[iOS/Android][GO2bank] [ODP 2.0] Go-Live</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BMAPP-21834</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Critical</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2022-06-16</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Dennis Wiles</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[GO2bank][Web] Add Domains to CSP Whitelisting</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-38699</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>2022-06-13</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Harold Finch</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>PO Review</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>https://jira.com/browse/proj-004</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>M110</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Rita Webb</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[COFO]  Research Extensibility of Current Mobile 2FA Service</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>[GBOS-61873] [COFO][SPIKE] Research Extensibility of Current Mobile 2FA Service - GDCJira (nextestate.com)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>Critical</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2022-06-16</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mark Sun</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[QA ONLY] SCC declines can re-apply after 30 days</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BMAPP-22159</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2022-06-16</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Mark Sun</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>[QA only] SCC declines can re-apply after 30 days</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-38697</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2022-06-14</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Sarath Krishnan</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>[GFT]Update the Utility Core API to get Bin info to add Program code</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GBOS-62197</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2022-05-20</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Megan Ackling</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Walgreens and CVS FeeSplit Setup for eCash Setup - GBOS</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/FEAS-24667</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2022-06-06</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sarath Krishnan</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>[GFT][MCsend]Create Adjusmentypes for Partner A2A and P2P</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GBOS-61750</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2022-06-02</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Tyler Penn</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ODP 2.0 : [TRIGGER FOR NTKey105] Tier Reinstated</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GBOS-62115</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>True</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>2022-05-25</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2022-05-23</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Megan Ackling</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>[QA Testing]ATM and AFT Limit Decrease for Regular Season - CoID 164</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GBOS-62061</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2022-06-07</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Smitha Jonnala</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>[WMMC] OAuth redirect is not working as expected</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/GB-80048</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2022-06-08</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Smitha Jonnala</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>BUX-37721: [Web] - [Server] [Go2bank and Chirp] Transactions API is not returning masked external account values for SCC transactions</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BUX-37721</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2022-06-08</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Smitha Jonnala</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>BMAPP-21860: [Server] [Go2bank and Chirp] Transactions API is not returning masked external account values for SCC transactions</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://pd.nextestate.com/browse/BMAPP-21860</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>M111</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>2022-06-23</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
         <is>
           <t>False</t>
         </is>

</xml_diff>

<commit_message>
Refactor code and fix the priority issue.
</commit_message>
<xml_diff>
--- a/sample/sorted.xlsx
+++ b/sample/sorted.xlsx
@@ -700,22 +700,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2022-06-15</t>
+          <t>2022-05-20</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mark Sun</t>
+          <t>Tyler Penn</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[SCC] Block non-SSN DDA applying for an SCC</t>
+          <t>[Web] [GO2bank] [ODP 2.0] Go-Live (Desktop browser)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/GBOS-62345</t>
+          <t>https://pd.nextestate.com/browse/BUX-37261</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -735,19 +735,19 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>N/A</t>
@@ -755,22 +755,22 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2022-06-22</t>
+          <t>2022-05-20</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -802,12 +802,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[Gateway] [GO2bank] [app upgrade] Set app force upgrade</t>
+          <t>[Web] [GO2bank] [ODP 2.0] Go-Live (Mobile browser)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/BUX-38827</t>
+          <t>https://pd.nextestate.com/browse/BUX-37262</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -827,7 +827,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -894,12 +894,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[Web] [GO2bank] [ODP 2.0] Go-Live (Desktop browser)</t>
+          <t>[iOS/Android][GO2bank] [ODP 2.0] Go-Live</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/BUX-37261</t>
+          <t>https://pd.nextestate.com/browse/BMAPP-21834</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2022-05-20</t>
+          <t>2022-06-02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -986,12 +986,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[Web] [GO2bank] [ODP 2.0] Go-Live (Mobile browser)</t>
+          <t>ODP 2.0 : [TRIGGER FOR NTKey105] Tier Reinstated</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/BUX-37262</t>
+          <t>https://pd.nextestate.com/browse/GBOS-62115</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>High</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -1021,27 +1021,27 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Middle</t>
-        </is>
-      </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1068,22 +1068,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2022-05-20</t>
+          <t>2022-06-07</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tyler Penn</t>
+          <t>Smitha Jonnala</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[iOS/Android][GO2bank] [ODP 2.0] Go-Live</t>
+          <t>[WMMC] OAuth redirect is not working as expected</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/BMAPP-21834</t>
+          <t>https://pd.nextestate.com/browse/GB-80048</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Critical</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1108,12 +1108,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1123,17 +1123,17 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -1160,22 +1160,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2022-06-16</t>
+          <t>2022-06-15</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Dennis Wiles</t>
+          <t>Mark Sun</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[GO2bank][Web] Add Domains to CSP Whitelisting</t>
+          <t>[SCC] Block non-SSN DDA applying for an SCC</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/BUX-38699</t>
+          <t>https://pd.nextestate.com/browse/GBOS-62345</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1190,22 +1190,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1215,17 +1215,17 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1252,22 +1252,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2022-06-13</t>
+          <t>2022-06-22</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rita Webb</t>
+          <t>Tyler Penn</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[COFO]  Research Extensibility of Current Mobile 2FA Service</t>
+          <t>[Gateway] [GO2bank] [app upgrade] Set app force upgrade</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[GBOS-61873] [COFO][SPIKE] Research Extensibility of Current Mobile 2FA Service - GDCJira (nextestate.com)</t>
+          <t>https://pd.nextestate.com/browse/BUX-38827</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Critical</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1307,22 +1307,22 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1344,22 +1344,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2022-06-16</t>
+          <t>2022-05-23</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mark Sun</t>
+          <t>Megan Ackling</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[QA ONLY] SCC declines can re-apply after 30 days</t>
+          <t>[QA Testing]ATM and AFT Limit Decrease for Regular Season - CoID 164</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/BMAPP-22159</t>
+          <t>https://pd.nextestate.com/browse/GBOS-62061</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1374,17 +1374,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1399,12 +1399,12 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1436,22 +1436,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2022-06-16</t>
+          <t>2022-06-14</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Mark Sun</t>
+          <t>Sarath Krishnan</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[QA only] SCC declines can re-apply after 30 days</t>
+          <t>[GFT]Update the Utility Core API to get Bin info to add Program code</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/BUX-38697</t>
+          <t>https://pd.nextestate.com/browse/GBOS-62197</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1491,12 +1491,12 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>High</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1528,22 +1528,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2022-06-14</t>
+          <t>2022-05-20</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sarath Krishnan</t>
+          <t>Megan Ackling</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[GFT]Update the Utility Core API to get Bin info to add Program code</t>
+          <t>Walgreens and CVS FeeSplit Setup for eCash Setup - GBOS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/GBOS-62197</t>
+          <t>https://pd.nextestate.com/browse/FEAS-24667</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1620,22 +1620,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2022-05-20</t>
+          <t>2022-06-06</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Megan Ackling</t>
+          <t>Sarath Krishnan</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Walgreens and CVS FeeSplit Setup for eCash Setup - GBOS</t>
+          <t>[GFT][MCsend]Create Adjusmentypes for Partner A2A and P2P</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/FEAS-24667</t>
+          <t>https://pd.nextestate.com/browse/GBOS-61750</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1712,22 +1712,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2022-06-06</t>
+          <t>2022-06-16</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sarath Krishnan</t>
+          <t>Dennis Wiles</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[GFT][MCsend]Create Adjusmentypes for Partner A2A and P2P</t>
+          <t>[GO2bank][Web] Add Domains to CSP Whitelisting</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/GBOS-61750</t>
+          <t>https://pd.nextestate.com/browse/BUX-38699</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1804,22 +1804,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2022-06-02</t>
+          <t>2022-06-13</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Tyler Penn</t>
+          <t>Rita Webb</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ODP 2.0 : [TRIGGER FOR NTKey105] Tier Reinstated</t>
+          <t>[COFO]  Research Extensibility of Current Mobile 2FA Service</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/GBOS-62115</t>
+          <t>[GBOS-61873] [COFO][SPIKE] Research Extensibility of Current Mobile 2FA Service - GDCJira (nextestate.com)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1829,17 +1829,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Middle</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1859,22 +1859,22 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
+          <t>Middle</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
           <t>Low</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1896,22 +1896,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2022-05-23</t>
+          <t>2022-06-16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Megan Ackling</t>
+          <t>Mark Sun</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>[QA Testing]ATM and AFT Limit Decrease for Regular Season - CoID 164</t>
+          <t>[QA ONLY] SCC declines can re-apply after 30 days</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/GBOS-62061</t>
+          <t>https://pd.nextestate.com/browse/BMAPP-22159</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1926,17 +1926,17 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>High</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1951,12 +1951,12 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1988,22 +1988,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2022-06-07</t>
+          <t>2022-06-16</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Smitha Jonnala</t>
+          <t>Mark Sun</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[WMMC] OAuth redirect is not working as expected</t>
+          <t>[QA only] SCC declines can re-apply after 30 days</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://pd.nextestate.com/browse/GB-80048</t>
+          <t>https://pd.nextestate.com/browse/BUX-38697</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -2023,12 +2023,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>High</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -2043,22 +2043,22 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Middle</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">

</xml_diff>